<commit_message>
established v1.2 and finished sensitivity
</commit_message>
<xml_diff>
--- a/Model_simulations/Exp1_run/Best_model_SDD.xlsx
+++ b/Model_simulations/Exp1_run/Best_model_SDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Documentos\github\BLT_IBM-Model\Model_simulations\Exp1_run\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B47893C-CFFA-4C9A-B9BD-C8C98553446E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC444859-D3DE-414A-95F9-A584C2920DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Estimate</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>p_traveling_z</t>
+  </si>
+  <si>
+    <t>Parameter</t>
   </si>
 </sst>
 </file>
@@ -84,7 +87,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -132,10 +135,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,7 +457,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="B2:E2"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -463,6 +467,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,7 +496,7 @@
       <c r="D2" s="2">
         <v>1167.7147603528524</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>0</v>
       </c>
     </row>
@@ -574,7 +581,7 @@
       <c r="D7" s="2">
         <v>5.9445047028237523</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>3.1384543722363567E-9</v>
       </c>
     </row>
@@ -591,7 +598,7 @@
       <c r="D8" s="2">
         <v>-1.9689864127353078</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>4.9059131682367495E-2</v>
       </c>
     </row>
@@ -616,16 +623,16 @@
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="3">
         <v>0.14717302467572091</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>5.042047409682269E-3</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="3">
         <v>29.189139394664121</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="3">
         <v>1.4551693890295878E-162</v>
       </c>
     </row>
@@ -642,7 +649,7 @@
       <c r="D11" s="2">
         <v>-3.0399581907673197</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="3">
         <v>2.3893417322076436E-3</v>
       </c>
     </row>
@@ -650,16 +657,16 @@
       <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="3">
         <v>-0.10858396364029792</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <v>5.0574218170525769E-3</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="3">
         <v>-21.470220908640709</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="3">
         <v>2.2237186997803488E-94</v>
       </c>
     </row>
@@ -676,7 +683,7 @@
       <c r="D13" s="2">
         <v>4.3819685270287856</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="3">
         <v>1.2220594667083413E-5</v>
       </c>
     </row>
@@ -693,7 +700,7 @@
       <c r="D14" s="2">
         <v>5.0524123794804634</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="3">
         <v>4.6606486423516302E-7</v>
       </c>
     </row>
@@ -710,7 +717,7 @@
       <c r="D15" s="2">
         <v>-3.4334277234082067</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="3">
         <v>6.0518945838890605E-4</v>
       </c>
     </row>
@@ -727,11 +734,12 @@
       <c r="D16" s="2">
         <v>2.721145067652182</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="3">
         <v>6.5483239771015733E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>